<commit_message>
Implementação da consulta de massa no Excel pelo nome do campo na planilha
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivos/CadastroUsuario.xlsx
+++ b/src/test/resources/arquivos/CadastroUsuario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anderson.santiago\Documents\automacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anderson.santiago\eclipse-workspace\DesafioAdvantage\src\test\resources\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>Mensagem</t>
+  </si>
+  <si>
+    <t>User name already exists</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,9 +469,10 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,8 +515,11 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -552,8 +562,11 @@
       <c r="N2" t="s">
         <v>21</v>
       </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="M3" s="3"/>
     </row>

</xml_diff>